<commit_message>
first draft of the analyses
</commit_message>
<xml_diff>
--- a/TableOR.xlsx
+++ b/TableOR.xlsx
@@ -92,7 +92,7 @@
     <t xml:space="preserve">home_care</t>
   </si>
   <si>
-    <t xml:space="preserve">Charlson_withoutage</t>
+    <t xml:space="preserve">Charlson_withage</t>
   </si>
   <si>
     <t xml:space="preserve">pod.family_friends</t>
@@ -461,13 +461,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>1.31</v>
+        <v>1.41</v>
       </c>
       <c r="C2" t="n">
-        <v>0.53</v>
+        <v>0.57</v>
       </c>
       <c r="D2" t="n">
-        <v>3.23</v>
+        <v>3.52</v>
       </c>
     </row>
     <row r="3">
@@ -475,13 +475,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>1.05</v>
+        <v>0.97</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>0.93</v>
       </c>
       <c r="D3" t="n">
-        <v>1.11</v>
+        <v>1.02</v>
       </c>
     </row>
     <row r="4">
@@ -489,13 +489,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>1.01</v>
+        <v>0.99</v>
       </c>
       <c r="C4" t="n">
-        <v>0.97</v>
+        <v>0.96</v>
       </c>
       <c r="D4" t="n">
-        <v>1.05</v>
+        <v>1.03</v>
       </c>
     </row>
     <row r="5">
@@ -503,13 +503,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>1.07</v>
+        <v>0.96</v>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>0.89</v>
       </c>
       <c r="D5" t="n">
-        <v>1.16</v>
+        <v>1.03</v>
       </c>
     </row>
     <row r="6">
@@ -517,13 +517,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>13.76</v>
+        <v>0.69</v>
       </c>
       <c r="C6" t="n">
-        <v>1.61</v>
+        <v>0.16</v>
       </c>
       <c r="D6" t="n">
-        <v>117.23</v>
+        <v>2.93</v>
       </c>
     </row>
     <row r="7">
@@ -531,13 +531,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>1.04</v>
+        <v>2.12</v>
       </c>
       <c r="C7" t="n">
-        <v>0.44</v>
+        <v>0.88</v>
       </c>
       <c r="D7" t="n">
-        <v>2.45</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="8">
@@ -545,13 +545,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>1.83</v>
       </c>
       <c r="C8" t="n">
-        <v>0.42</v>
+        <v>0.76</v>
       </c>
       <c r="D8" t="n">
-        <v>2.37</v>
+        <v>4.41</v>
       </c>
     </row>
     <row r="9">
@@ -559,13 +559,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>0.39</v>
+        <v>2.98</v>
       </c>
       <c r="C9" t="n">
-        <v>0.04</v>
+        <v>0.32</v>
       </c>
       <c r="D9" t="n">
-        <v>3.59</v>
+        <v>27.75</v>
       </c>
     </row>
     <row r="10">
@@ -573,13 +573,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>1.06</v>
+        <v>1.78</v>
       </c>
       <c r="C10" t="n">
-        <v>0.41</v>
+        <v>0.7</v>
       </c>
       <c r="D10" t="n">
-        <v>2.56</v>
+        <v>1.16</v>
       </c>
     </row>
     <row r="11">
@@ -587,13 +587,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>1.2</v>
+        <v>1.55</v>
       </c>
       <c r="C11" t="n">
-        <v>0.43</v>
+        <v>0.57</v>
       </c>
       <c r="D11" t="n">
-        <v>3.35</v>
+        <v>4.19</v>
       </c>
     </row>
     <row r="12">
@@ -601,10 +601,10 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>1.5</v>
+        <v>0.85</v>
       </c>
       <c r="C12" t="n">
-        <v>0.2</v>
+        <v>0.11</v>
       </c>
       <c r="D12" t="n">
         <v>0</v>
@@ -615,13 +615,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>118848596299903672516608</v>
+        <v>0.94</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
-      </c>
-      <c r="D13" t="e">
-        <v>#NUM!</v>
+        <v>0.4</v>
+      </c>
+      <c r="D13" t="n">
+        <v>1.46</v>
       </c>
     </row>
     <row r="14">
@@ -629,13 +629,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>108.8</v>
+        <v>1.31</v>
       </c>
       <c r="C14" t="n">
-        <v>24.32</v>
+        <v>0.56</v>
       </c>
       <c r="D14" t="n">
-        <v>0.4</v>
+        <v>1.18</v>
       </c>
     </row>
     <row r="15">
@@ -643,13 +643,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>7.05</v>
+        <v>1.16</v>
       </c>
       <c r="C15" t="n">
-        <v>1.79</v>
+        <v>0.35</v>
       </c>
       <c r="D15" t="n">
-        <v>27.8</v>
+        <v>3.85</v>
       </c>
     </row>
     <row r="16">
@@ -657,13 +657,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>3.67</v>
+        <v>0.88</v>
       </c>
       <c r="C16" t="n">
-        <v>0.86</v>
+        <v>0.22</v>
       </c>
       <c r="D16" t="n">
-        <v>15.72</v>
+        <v>3.49</v>
       </c>
     </row>
     <row r="17">
@@ -671,13 +671,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>1.51</v>
+        <v>0.72</v>
       </c>
       <c r="C17" t="n">
-        <v>1.01</v>
+        <v>0.49</v>
       </c>
       <c r="D17" t="n">
-        <v>2.26</v>
+        <v>1.08</v>
       </c>
     </row>
     <row r="18">
@@ -685,13 +685,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>1.2</v>
+        <v>0.98</v>
       </c>
       <c r="C18" t="n">
-        <v>0.77</v>
+        <v>0.64</v>
       </c>
       <c r="D18" t="n">
-        <v>1.86</v>
+        <v>1.51</v>
       </c>
     </row>
     <row r="19">
@@ -699,13 +699,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>1.02</v>
+        <v>0.79</v>
       </c>
       <c r="C19" t="n">
-        <v>0.82</v>
+        <v>0.62</v>
       </c>
       <c r="D19" t="n">
-        <v>1.26</v>
+        <v>1.01</v>
       </c>
     </row>
     <row r="20">
@@ -713,13 +713,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>1.08</v>
+        <v>1.24</v>
       </c>
       <c r="C20" t="n">
-        <v>0.72</v>
+        <v>0.84</v>
       </c>
       <c r="D20" t="n">
-        <v>1.6</v>
+        <v>1.85</v>
       </c>
     </row>
     <row r="21">
@@ -727,13 +727,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>0.99</v>
+        <v>0.94</v>
       </c>
       <c r="C21" t="n">
-        <v>0.79</v>
+        <v>0.74</v>
       </c>
       <c r="D21" t="n">
-        <v>1.24</v>
+        <v>1.18</v>
       </c>
     </row>
     <row r="22">
@@ -741,10 +741,10 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>0.81</v>
+        <v>0</v>
       </c>
       <c r="C22" t="n">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="D22" t="n">
         <v>0</v>
@@ -755,13 +755,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>1.04</v>
+        <v>18</v>
       </c>
       <c r="C23" t="n">
-        <v>0.44</v>
+        <v>4.93</v>
       </c>
       <c r="D23" t="n">
-        <v>2.45</v>
+        <v>65.75</v>
       </c>
     </row>
     <row r="24">
@@ -769,13 +769,13 @@
         <v>26</v>
       </c>
       <c r="B24" t="n">
-        <v>1.09</v>
+        <v>1.04</v>
       </c>
       <c r="C24" t="n">
-        <v>0.72</v>
+        <v>0.79</v>
       </c>
       <c r="D24" t="n">
-        <v>1.66</v>
+        <v>1.36</v>
       </c>
     </row>
     <row r="25">
@@ -783,13 +783,13 @@
         <v>27</v>
       </c>
       <c r="B25" t="n">
-        <v>0.86</v>
+        <v>1.05</v>
       </c>
       <c r="C25" t="n">
-        <v>0.37</v>
+        <v>0.46</v>
       </c>
       <c r="D25" t="n">
-        <v>1.98</v>
+        <v>2.38</v>
       </c>
     </row>
     <row r="26">
@@ -797,13 +797,13 @@
         <v>28</v>
       </c>
       <c r="B26" t="n">
-        <v>29197420.23</v>
+        <v>0.66</v>
       </c>
       <c r="C26" t="n">
-        <v>0</v>
+        <v>0.12</v>
       </c>
       <c r="D26" t="n">
-        <v>2.24</v>
+        <v>1.16</v>
       </c>
     </row>
     <row r="27">
@@ -811,13 +811,13 @@
         <v>29</v>
       </c>
       <c r="B27" t="n">
-        <v>3664062.73</v>
+        <v>0</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>2.4</v>
+        <v>1.11</v>
       </c>
     </row>
     <row r="28">
@@ -825,13 +825,13 @@
         <v>30</v>
       </c>
       <c r="B28" t="n">
-        <v>109397506.63</v>
+        <v>0.7</v>
       </c>
       <c r="C28" t="n">
-        <v>0</v>
+        <v>0.22</v>
       </c>
       <c r="D28" t="n">
-        <v>1.68</v>
+        <v>1.14</v>
       </c>
     </row>
     <row r="29">
@@ -839,13 +839,13 @@
         <v>31</v>
       </c>
       <c r="B29" t="n">
-        <v>1.14</v>
+        <v>0.83</v>
       </c>
       <c r="C29" t="n">
-        <v>0.8</v>
+        <v>0.59</v>
       </c>
       <c r="D29" t="n">
-        <v>1.62</v>
+        <v>1.18</v>
       </c>
     </row>
     <row r="30">
@@ -853,13 +853,13 @@
         <v>32</v>
       </c>
       <c r="B30" t="n">
-        <v>1.18</v>
+        <v>1.08</v>
       </c>
       <c r="C30" t="n">
-        <v>0.51</v>
+        <v>0.47</v>
       </c>
       <c r="D30" t="n">
-        <v>2.72</v>
+        <v>2.46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>